<commit_message>
Fixed test cases and added new bug reports
</commit_message>
<xml_diff>
--- a/Тест-кейсы.xlsx
+++ b/Тест-кейсы.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -76,7 +76,7 @@
     <t>TS-01</t>
   </si>
   <si>
-    <t>Проверка входа с корректными учетными данными</t>
+    <t>Вход с корректными учетными данными</t>
   </si>
   <si>
     <t>Login page</t>
@@ -85,7 +85,7 @@
     <t>Пользователь не зашел в систему</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Открыть форма входа (https://demo.applitools.com/index.html)
+    <t xml:space="preserve">1. Открыть форму входа (https://demo.applitools.com/index.html)
 2. Ввести корректное имя пользователя
 3. Ввести корректный пароль
 4. Нажать кнопку "Sign in"
@@ -115,16 +115,16 @@
     <t>TS-02</t>
   </si>
   <si>
-    <t>Проверка входа с пустыми полями</t>
-  </si>
-  <si>
-    <t>1. Открыть форма входа (https://demo.applitools.com/index.html)
-2. Оставить поля пустыми
+    <t>Вход с незаполненными полями</t>
+  </si>
+  <si>
+    <t>1. Открыть форму входа (https://demo.applitools.com/index.html)
+2. Оставить поля незаполненными
 3. Нажать кнопку "Sign in"</t>
   </si>
   <si>
-    <t>1. Форма открывается
-2. Поля пустые
+    <t>1. Форма открыта
+2. Поля оставлены незаполненными 
 3. Перевод на главную страницу не осуществляется</t>
   </si>
   <si>
@@ -141,23 +141,25 @@
     <t>TS-03</t>
   </si>
   <si>
-    <t>Проверка "Remember me" при успешном входе</t>
-  </si>
-  <si>
-    <t>1. Открыть форма входа (https://demo.applitools.com/index.html)
+    <t>Включение чекбокса "Remember me" при успешном входе</t>
+  </si>
+  <si>
+    <t>1. Открыть форму входа (https://demo.applitools.com/index.html)
 2. Ввести имя пользователя
 3. Ввести пароль
-4. Поставить флажок "Remember me"
+4. Включить чекбокс "Remember me"
 5. Нажать кнопку "Sign in"
-6. Выйти и открыть заново</t>
-  </si>
-  <si>
-    <t>1. Форма открывается
+6. Закрыть главную страницу
+7. Открыть главную страницу</t>
+  </si>
+  <si>
+    <t>1. Форма открыта
 2. Имя введено
 3. Пароль введен
-4. Флажок ставится
+4. Чекбокс включен
 5. Перевод на главную страницу
-6. Пользователь сразу перенаправлен на главную страницу</t>
+6. Главная страница закрыта
+7. Пользователь перенаправлен на главную страницу</t>
   </si>
   <si>
     <t>Сайт не запомнил пользователя и предлагает авторизоваться</t>
@@ -166,7 +168,7 @@
     <t>TS-04</t>
   </si>
   <si>
-    <t>Проверка регистрации с корректными данными</t>
+    <t>Регистрация с корректными данными</t>
   </si>
   <si>
     <t>Registration page</t>
@@ -181,7 +183,7 @@
   </si>
   <si>
     <t>1. Форма открывается
-2. Поля заполнены валидными данными
+2. Поля заполнены 
 3. Пользователь зарегистрирован</t>
   </si>
   <si>
@@ -191,12 +193,36 @@
     <t>TS-05</t>
   </si>
   <si>
-    <t>Проверка регистрации без символа "@" в поле "Email address"</t>
+    <t>Регистрация без символа "@" в поле "Email address"</t>
   </si>
   <si>
     <t>1.Открыть форму регистрации (https://practicesoftwaretesting.com/auth/register)
-2.Заполнить поля валидными данными
+2.Заполнить поля
 3. В поле "Email address" указать адрес без "@"
+4. Нажать кнопку "register"</t>
+  </si>
+  <si>
+    <t>1. Форма открыта
+2. Поля заполнены 
+3. Сообщение о неправильно заполненном поле
+4. Регистрация не осуществляется</t>
+  </si>
+  <si>
+    <t>Сайт выделяет красным цветом неверно заполненное поле, но не сообщает что неправильно</t>
+  </si>
+  <si>
+    <t>Средний</t>
+  </si>
+  <si>
+    <t>TS-06</t>
+  </si>
+  <si>
+    <t>Ввод пароля без цифр и с длинной меньше 8 символов в форме регистрации</t>
+  </si>
+  <si>
+    <t>1.Открыть форму регистрации (https://practicesoftwaretesting.com/auth/register)
+2.Заполнить поля
+3.В поле "Password" написать пароль без цифр и длинной меньше 8 символов
 4. Нажать кнопку "register"</t>
   </si>
   <si>
@@ -206,31 +232,13 @@
 4. Регистрация не осуществляется</t>
   </si>
   <si>
-    <t>Сайт выделяет красным цветом неверно заполненное поле, но не указывает причину ошибки</t>
-  </si>
-  <si>
-    <t>Средний</t>
-  </si>
-  <si>
-    <t>TS-06</t>
-  </si>
-  <si>
-    <t>Ввод пароля без цифр и с длинной меньше 8 символов в форме регистрации</t>
-  </si>
-  <si>
-    <t>1.Открыть форму регистрации (https://practicesoftwaretesting.com/auth/register)
-2.Заполнить поля
-3.В поле "Password" написать пароль без цифр и длинной меньше 8 символов
-4. Нажать кнопку "register"</t>
-  </si>
-  <si>
-    <t>Сайт выделяет красным цветом неверно заполненное поле,  указывает причину ошибки</t>
+    <t>Сайт сообщает о неправильно заполненном поле</t>
   </si>
   <si>
     <t>TS-07</t>
   </si>
   <si>
-    <t>Проверка смены языков на главной странице</t>
+    <t>Смена языков на главной странице</t>
   </si>
   <si>
     <t>Header</t>
@@ -308,7 +316,7 @@
 5. Выбрать "My favorites"</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Открыть главную страницу
+    <t xml:space="preserve">1. Открыта главная страница
 2. Переход осуществляется
 3. Товар добавлен в избранное
 4. Переход на страницу пользователя
@@ -503,7 +511,7 @@
   </si>
   <si>
     <t>1. Сообщение записано 
-2. Сообщение отправляется. Код в сообщение экранируется и не исполняется</t>
+2. Сообщение отправленно. Код в сообщение экранируется и не исполняется</t>
   </si>
   <si>
     <t xml:space="preserve">Чат не экранирует написанный код. Код исполняется </t>
@@ -1594,10 +1602,10 @@
         <v>48</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>18</v>
@@ -1611,23 +1619,23 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>18</v>
@@ -1641,25 +1649,25 @@
     </row>
     <row r="10">
       <c r="A10" s="7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>18</v>
@@ -1673,25 +1681,25 @@
     </row>
     <row r="11">
       <c r="A11" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>18</v>
@@ -1706,7 +1714,7 @@
     <row r="12" ht="30.0" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="11" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1719,31 +1727,31 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>27</v>
@@ -1751,31 +1759,31 @@
     </row>
     <row r="14">
       <c r="A14" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>27</v>
@@ -1783,31 +1791,31 @@
     </row>
     <row r="15">
       <c r="A15" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>27</v>
@@ -1815,31 +1823,31 @@
     </row>
     <row r="16">
       <c r="A16" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>27</v>
@@ -1847,31 +1855,31 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>27</v>
@@ -1879,31 +1887,31 @@
     </row>
     <row r="18">
       <c r="A18" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>18</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J18" s="8" t="s">
         <v>27</v>
@@ -1911,31 +1919,31 @@
     </row>
     <row r="19">
       <c r="A19" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J19" s="8" t="s">
         <v>27</v>
@@ -1944,7 +1952,7 @@
     <row r="20" ht="30.0" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1957,25 +1965,25 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H21" s="9" t="s">
         <v>18</v>
@@ -1984,30 +1992,30 @@
         <v>19</v>
       </c>
       <c r="J21" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>18</v>
@@ -2016,30 +2024,30 @@
         <v>19</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H23" s="9" t="s">
         <v>18</v>
@@ -2048,30 +2056,30 @@
         <v>19</v>
       </c>
       <c r="J23" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H24" s="9" t="s">
         <v>18</v>
@@ -2080,30 +2088,30 @@
         <v>19</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H25" s="10" t="s">
         <v>26</v>
@@ -2112,30 +2120,30 @@
         <v>45</v>
       </c>
       <c r="J25" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H26" s="9" t="s">
         <v>18</v>
@@ -2144,12 +2152,12 @@
         <v>45</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="7" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -2160,12 +2168,12 @@
       <c r="H27" s="15"/>
       <c r="I27" s="15"/>
       <c r="J27" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="7" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -2176,7 +2184,7 @@
       <c r="H28" s="15"/>
       <c r="I28" s="15"/>
       <c r="J28" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
@@ -13822,8 +13830,8 @@
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B12:J12"/>
     <mergeCell ref="B20:J20"/>
-    <mergeCell ref="B12:J12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>

</xml_diff>